<commit_message>
Add testing for shift instructions in AST.
</commit_message>
<xml_diff>
--- a/docs/InstructionChecklist.xlsx
+++ b/docs/InstructionChecklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t>Instruction</t>
   </si>
@@ -497,7 +497,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,9 @@
         <v>37</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -726,7 +728,9 @@
         <v>37</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -737,7 +741,9 @@
         <v>37</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -748,7 +754,9 @@
         <v>37</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -759,7 +767,9 @@
         <v>37</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Tokeniser and AST with new instructions.
</commit_message>
<xml_diff>
--- a/docs/InstructionChecklist.xlsx
+++ b/docs/InstructionChecklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
   <si>
     <t>Instruction</t>
   </si>
@@ -497,7 +497,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +563,9 @@
         <v>37</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -832,7 +834,9 @@
         <v>37</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -843,7 +847,9 @@
         <v>37</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -872,16 +878,22 @@
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>

</xml_diff>

<commit_message>
Added tests and implemented instructions
</commit_message>
<xml_diff>
--- a/docs/InstructionChecklist.xlsx
+++ b/docs/InstructionChecklist.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YoussefRizk/Desktop/HLP/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="22260" windowHeight="12640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="40">
   <si>
     <t>Instruction</t>
   </si>
@@ -144,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -496,20 +504,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,7 +537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -540,9 +548,11 @@
       <c r="D2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -553,9 +563,11 @@
       <c r="D3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -566,9 +578,11 @@
       <c r="D4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -577,9 +591,11 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -590,9 +606,11 @@
       <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -603,9 +621,11 @@
       <c r="D7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -616,9 +636,11 @@
       <c r="D8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -629,9 +651,11 @@
       <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -642,9 +666,11 @@
       <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -655,9 +681,11 @@
       <c r="D11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -668,9 +696,11 @@
       <c r="D12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -681,9 +711,11 @@
       <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -694,9 +726,11 @@
       <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
@@ -707,9 +741,11 @@
       <c r="D15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -720,9 +756,11 @@
       <c r="D16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -733,9 +771,11 @@
       <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -746,9 +786,11 @@
       <c r="D18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>22</v>
       </c>
@@ -759,9 +801,11 @@
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -772,9 +816,11 @@
       <c r="D20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -785,9 +831,11 @@
       <c r="D21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -798,9 +846,11 @@
       <c r="D22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -811,9 +861,11 @@
       <c r="D23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
@@ -824,9 +876,11 @@
       <c r="D24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
@@ -837,9 +891,11 @@
       <c r="D25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -850,9 +906,11 @@
       <c r="D26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
@@ -861,9 +919,11 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
@@ -872,9 +932,11 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -885,9 +947,11 @@
       <c r="D29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
@@ -898,7 +962,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
@@ -907,7 +971,7 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -916,7 +980,7 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
@@ -925,7 +989,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
@@ -934,44 +998,44 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>

</xml_diff>

<commit_message>
Update Tokeniser to support DCD, FILL, EQU and END.
</commit_message>
<xml_diff>
--- a/docs/InstructionChecklist.xlsx
+++ b/docs/InstructionChecklist.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\High Level Programming\ARM-Emulator\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,139 +24,136 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="41">
-  <si>
-    <t xml:space="preserve">Instruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tokeniser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InstructionsInterfaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fully Tested in pipeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MVN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDR (pseudo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LSL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LSR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RRX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EQU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FILL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">END</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="41">
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>Tokeniser</t>
+  </si>
+  <si>
+    <t>Parser</t>
+  </si>
+  <si>
+    <t>AST</t>
+  </si>
+  <si>
+    <t>InstructionsInterfaces</t>
+  </si>
+  <si>
+    <t>Fully Tested in pipeline</t>
+  </si>
+  <si>
+    <t>MOV</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>MVN</t>
+  </si>
+  <si>
+    <t>ADR</t>
+  </si>
+  <si>
+    <t>LDR (pseudo)</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>SBC</t>
+  </si>
+  <si>
+    <t>RSB</t>
+  </si>
+  <si>
+    <t>RSC</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>EOR</t>
+  </si>
+  <si>
+    <t>BIC</t>
+  </si>
+  <si>
+    <t>ORR</t>
+  </si>
+  <si>
+    <t>LSL</t>
+  </si>
+  <si>
+    <t>LSR</t>
+  </si>
+  <si>
+    <t>ASR</t>
+  </si>
+  <si>
+    <t>ROR</t>
+  </si>
+  <si>
+    <t>RRX</t>
+  </si>
+  <si>
+    <t>CMP</t>
+  </si>
+  <si>
+    <t>CMN</t>
+  </si>
+  <si>
+    <t>TST</t>
+  </si>
+  <si>
+    <t>TEQ</t>
+  </si>
+  <si>
+    <t>LDR</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>LDM</t>
+  </si>
+  <si>
+    <t>STM</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>DCD</t>
+  </si>
+  <si>
+    <t>EQU</t>
+  </si>
+  <si>
+    <t>FILL</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -161,22 +162,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -200,14 +186,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FFDDDDDD"/>
       </left>
@@ -223,57 +209,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -332,34 +287,342 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col min="1" max="1" width="22"/>
+    <col min="2" max="2" width="9.7109375"/>
+    <col min="3" max="3" width="8.5703125"/>
+    <col min="4" max="4" width="13.140625"/>
+    <col min="5" max="5" width="20.7109375"/>
+    <col min="6" max="6" width="23.42578125" style="1"/>
+    <col min="7" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -379,7 +642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -394,7 +657,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -409,7 +672,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -424,7 +687,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -435,7 +698,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -450,7 +713,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -465,7 +728,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -480,7 +743,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -495,7 +758,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -510,7 +773,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -525,7 +788,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -540,7 +803,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -555,7 +818,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -570,7 +833,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -585,7 +848,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -600,7 +863,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -615,7 +878,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -630,7 +893,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -645,7 +908,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -660,7 +923,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -675,7 +938,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -690,7 +953,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -705,7 +968,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -720,7 +983,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
@@ -735,7 +998,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
@@ -750,7 +1013,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
@@ -763,7 +1026,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
@@ -776,7 +1039,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -791,7 +1054,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
@@ -804,50 +1067,53 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add FILL instruction to AST
</commit_message>
<xml_diff>
--- a/docs/InstructionChecklist.xlsx
+++ b/docs/InstructionChecklist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
   <si>
     <t>Instruction</t>
   </si>
@@ -608,7 +608,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1023,9 @@
       <c r="C27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1036,7 +1038,9 @@
       <c r="C28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1074,8 +1078,12 @@
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,8 +1093,12 @@
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1096,8 +1108,12 @@
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1107,8 +1123,12 @@
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E34" s="1"/>
     </row>
     <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>